<commit_message>
loop for check ap
</commit_message>
<xml_diff>
--- a/Morning Check List.xlsx
+++ b/Morning Check List.xlsx
@@ -37,10 +37,10 @@
     <t>Down</t>
   </si>
   <si>
+    <t>BSSID STATUS</t>
+  </si>
+  <si>
     <t>Floor</t>
-  </si>
-  <si>
-    <t>BSSID STATUS</t>
   </si>
   <si>
     <t>@Enterprise</t>
@@ -501,9 +501,7 @@
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -515,7 +513,9 @@
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
@@ -548,9 +548,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:K1"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -568,9 +567,7 @@
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -582,7 +579,9 @@
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
@@ -615,9 +614,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:K1"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -635,9 +633,7 @@
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -649,7 +645,9 @@
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
@@ -682,9 +680,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:K1"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
edit code main and template 2024-02-28
</commit_message>
<xml_diff>
--- a/Morning Check List.xlsx
+++ b/Morning Check List.xlsx
@@ -428,7 +428,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -476,6 +476,26 @@
       </c>
       <c r="F3" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>282</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>358</v>
+      </c>
+      <c r="D4" s="1">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1">
+        <v>155</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>